<commit_message>
Mango pine apple sal nego
</commit_message>
<xml_diff>
--- a/Shared Texts files/pam docs/pammi.xlsx
+++ b/Shared Texts files/pam docs/pammi.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\sharedThingsGit\commonFiles\Shared Texts files\pam docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\navanit\Documents\personalGit\commonFiles\Shared Texts files\pam docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD3E1850-DA49-4D00-8717-8140AFC4B642}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89537C76-E680-49B0-A20E-2BFAD2D46824}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{961402BA-B10A-4D6B-B6EB-3F1599D4CF9C}"/>
   </bookViews>
@@ -36,8 +36,53 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={3AE5FFB7-E6A8-4346-B5D1-3B952D1B6090}</author>
+    <author>tc={EA29DB3E-C8F1-47B5-BDBD-5E0195108BA5}</author>
+    <author>tc={010FB3D0-4785-4FB6-A179-776F73C1B377}</author>
+    <author>tc={424D6C1E-3801-4518-9FD9-10B7A90F8708}</author>
+  </authors>
+  <commentList>
+    <comment ref="F3" authorId="0" shapeId="0" xr:uid="{3AE5FFB7-E6A8-4346-B5D1-3B952D1B6090}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    5500 + 440</t>
+      </text>
+    </comment>
+    <comment ref="F4" authorId="1" shapeId="0" xr:uid="{EA29DB3E-C8F1-47B5-BDBD-5E0195108BA5}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    5500 * 12</t>
+      </text>
+    </comment>
+    <comment ref="F6" authorId="2" shapeId="0" xr:uid="{010FB3D0-4785-4FB6-A179-776F73C1B377}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    440 * 12</t>
+      </text>
+    </comment>
+    <comment ref="G7" authorId="3" shapeId="0" xr:uid="{424D6C1E-3801-4518-9FD9-10B7A90F8708}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    If you include 13th Month Pay.</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="28">
   <si>
     <t>Current</t>
   </si>
@@ -109,16 +154,71 @@
   </si>
   <si>
     <t xml:space="preserve">what we want </t>
+  </si>
+  <si>
+    <r>
+      <t>Entire salary paid in monthly instalments (incl. holiday allowance</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> and 13th month</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Annual salary excl. Holiday allowance </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>excl 13th month</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Annual salary included Holiday allowance </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>and 13th month</t>
+    </r>
+  </si>
+  <si>
+    <t>Net monthly</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="[$€-2]\ #,##0;[Red]\-[$€-2]\ #,##0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="[$€-2]\ #,##0;[Red]\-[$€-2]\ #,##0"/>
+    <numFmt numFmtId="169" formatCode="[$€-2]\ #,##0.00;[Red]\-[$€-2]\ #,##0.00"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -166,6 +266,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -281,7 +387,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -305,12 +411,6 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -321,17 +421,11 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -349,14 +443,30 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -372,6 +482,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Navanit Kamble" id="{6921EA79-0C74-48BA-89CC-5A7B7A191425}" userId="S::navanit.kamble@eurofiber.com::6a14f368-9837-42b7-b363-11e6a670e3c2" providerId="AD"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -689,6 +805,23 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="F3" dT="2024-06-05T08:12:55.23" personId="{6921EA79-0C74-48BA-89CC-5A7B7A191425}" id="{3AE5FFB7-E6A8-4346-B5D1-3B952D1B6090}">
+    <text>5500 + 440</text>
+  </threadedComment>
+  <threadedComment ref="F4" dT="2024-06-05T08:14:21.48" personId="{6921EA79-0C74-48BA-89CC-5A7B7A191425}" id="{EA29DB3E-C8F1-47B5-BDBD-5E0195108BA5}">
+    <text>5500 * 12</text>
+  </threadedComment>
+  <threadedComment ref="F6" dT="2024-06-05T08:12:25.52" personId="{6921EA79-0C74-48BA-89CC-5A7B7A191425}" id="{010FB3D0-4785-4FB6-A179-776F73C1B377}">
+    <text>440 * 12</text>
+  </threadedComment>
+  <threadedComment ref="G7" dT="2024-06-05T08:20:45.03" personId="{6921EA79-0C74-48BA-89CC-5A7B7A191425}" id="{424D6C1E-3801-4518-9FD9-10B7A90F8708}">
+    <text>If you include 13th Month Pay.</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69F0088F-47E9-4A1E-9DC5-AD2CC6E1416B}">
   <dimension ref="A1:F12"/>
@@ -707,16 +840,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="11"/>
-      <c r="B1" s="12" t="s">
+      <c r="A1" s="9"/>
+      <c r="B1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="10" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
-      <c r="F1" s="18"/>
+      <c r="F1" s="14"/>
     </row>
     <row r="2" spans="1:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
@@ -728,7 +861,7 @@
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
-      <c r="F2" s="19">
+      <c r="F2" s="15">
         <v>5500</v>
       </c>
     </row>
@@ -742,7 +875,7 @@
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
-      <c r="F3" s="19">
+      <c r="F3" s="15">
         <v>5940</v>
       </c>
     </row>
@@ -756,7 +889,7 @@
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
-      <c r="F4" s="20">
+      <c r="F4" s="16">
         <v>66000</v>
       </c>
     </row>
@@ -770,7 +903,7 @@
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
-      <c r="F5" s="18" t="s">
+      <c r="F5" s="14" t="s">
         <v>22</v>
       </c>
     </row>
@@ -784,7 +917,7 @@
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
-      <c r="F6" s="20">
+      <c r="F6" s="16">
         <v>5280</v>
       </c>
     </row>
@@ -798,7 +931,7 @@
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="19">
+      <c r="F7" s="15">
         <v>71280</v>
       </c>
     </row>
@@ -810,21 +943,21 @@
       <c r="C8" s="4"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
-      <c r="F8" s="18"/>
-    </row>
-    <row r="9" spans="1:6" s="17" customFormat="1" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="13" t="s">
+      <c r="F8" s="14"/>
+    </row>
+    <row r="9" spans="1:6" s="13" customFormat="1" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14" t="s">
+      <c r="B9" s="12"/>
+      <c r="C9" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="15" t="s">
+      <c r="D9" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="16"/>
-      <c r="F9" s="20">
+      <c r="E9" s="27"/>
+      <c r="F9" s="16">
         <v>5500</v>
       </c>
     </row>
@@ -836,11 +969,11 @@
       <c r="C10" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="D10" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="9"/>
-      <c r="F10" s="18" t="s">
+      <c r="E10" s="29"/>
+      <c r="F10" s="14" t="s">
         <v>22</v>
       </c>
     </row>
@@ -852,7 +985,7 @@
       <c r="C11" s="4"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
-      <c r="F11" s="18" t="s">
+      <c r="F11" s="14" t="s">
         <v>22</v>
       </c>
     </row>
@@ -866,7 +999,7 @@
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
-      <c r="F12" s="21">
+      <c r="F12" s="17">
         <v>76780</v>
       </c>
     </row>
@@ -881,11 +1014,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD9F65E5-D0EE-418F-AE79-B905BE25108F}">
-  <dimension ref="A1:G12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD9F65E5-D0EE-418F-AE79-B905BE25108F}">
+  <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" zoomScale="134" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -895,185 +1028,194 @@
     <col min="4" max="5" width="0" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="17.44140625" customWidth="1"/>
     <col min="7" max="7" width="15.77734375" customWidth="1"/>
+    <col min="8" max="8" width="17.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="30"/>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="25"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A2" s="22" t="s">
+      <c r="H1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15" x14ac:dyDescent="0.3">
+      <c r="A2" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22" t="s">
+      <c r="B2" s="18"/>
+      <c r="C2" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="19">
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="15">
         <v>5500</v>
       </c>
-      <c r="G2" s="18"/>
-    </row>
-    <row r="3" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A3" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22" t="s">
+      <c r="G2" s="15">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15" x14ac:dyDescent="0.3">
+      <c r="A3" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="18"/>
+      <c r="C3" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="19">
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="15">
         <v>5940</v>
       </c>
-      <c r="G3" s="18"/>
-    </row>
-    <row r="4" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A4" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="22"/>
-      <c r="C4" s="22" t="s">
+      <c r="G3" s="14"/>
+      <c r="H3" s="32">
+        <v>4665.8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15" x14ac:dyDescent="0.3">
+      <c r="A4" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="18"/>
+      <c r="C4" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="19">
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="15">
         <v>66000</v>
       </c>
-      <c r="G4" s="18"/>
-    </row>
-    <row r="5" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+      <c r="G4" s="14"/>
+    </row>
+    <row r="5" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A5" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="22"/>
-      <c r="C5" s="22" t="s">
+      <c r="B5" s="18"/>
+      <c r="C5" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="18" t="s">
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="G5" s="19">
+      <c r="G5" s="15">
         <v>5500</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A6" s="22" t="s">
+    <row r="6" spans="1:8" ht="15" x14ac:dyDescent="0.3">
+      <c r="A6" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="22"/>
-      <c r="C6" s="22" t="s">
+      <c r="B6" s="18"/>
+      <c r="C6" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="19">
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="15">
         <v>5280</v>
       </c>
-      <c r="G6" s="18"/>
-    </row>
-    <row r="7" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A7" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="24"/>
-      <c r="C7" s="24" t="s">
+      <c r="G6" s="14"/>
+    </row>
+    <row r="7" spans="1:8" ht="15" x14ac:dyDescent="0.3">
+      <c r="A7" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="19">
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="15">
         <v>71280</v>
       </c>
-      <c r="G7" s="19">
+      <c r="G7" s="15">
         <v>76780</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A8" s="22" t="s">
+    <row r="8" spans="1:8" ht="15" x14ac:dyDescent="0.3">
+      <c r="A8" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="22"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-    </row>
-    <row r="9" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A9" s="25" t="s">
+      <c r="B8" s="18"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+    </row>
+    <row r="9" spans="1:8" ht="15" x14ac:dyDescent="0.3">
+      <c r="A9" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="25"/>
-      <c r="C9" s="25" t="s">
+      <c r="B9" s="21"/>
+      <c r="C9" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="26" t="s">
+      <c r="D9" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="26"/>
-      <c r="F9" s="19">
+      <c r="E9" s="30"/>
+      <c r="F9" s="15">
         <v>5500</v>
       </c>
-      <c r="G9" s="18"/>
-    </row>
-    <row r="10" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A10" s="24" t="s">
+      <c r="G9" s="14"/>
+    </row>
+    <row r="10" spans="1:8" ht="15" x14ac:dyDescent="0.3">
+      <c r="A10" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="24"/>
-      <c r="C10" s="24" t="s">
+      <c r="B10" s="20"/>
+      <c r="C10" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="27" t="s">
+      <c r="D10" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="27"/>
-      <c r="F10" s="18" t="s">
+      <c r="E10" s="31"/>
+      <c r="F10" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="G10" s="18"/>
-    </row>
-    <row r="11" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A11" s="22" t="s">
+      <c r="G10" s="14"/>
+    </row>
+    <row r="11" spans="1:8" ht="15" x14ac:dyDescent="0.3">
+      <c r="A11" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="22"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="23"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="18" t="s">
+      <c r="B11" s="18"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="G11" s="18"/>
-    </row>
-    <row r="12" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="28" t="s">
+      <c r="G11" s="14"/>
+    </row>
+    <row r="12" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="28"/>
-      <c r="C12" s="28" t="s">
+      <c r="B12" s="23"/>
+      <c r="C12" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="29"/>
-      <c r="E12" s="29"/>
-      <c r="F12" s="21">
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="17">
         <v>76780</v>
       </c>
-      <c r="G12" s="18"/>
+      <c r="G12" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1081,5 +1223,6 @@
     <mergeCell ref="D10:E10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>